<commit_message>
cambio en data driven para prueba
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/PolicyIssuanceParserMassive.xlsx
+++ b/src/test/resources/datadriven/PolicyIssuanceParserMassive.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dumartinez\Documents\Automatización Acsel-e\Acsel-e\src\test\resources\datadriven\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\GitHub\Acsel-e\Acsel-e\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18108EB4-EB75-47F1-9059-52FC659C676B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3261872-E942-4D51-956C-F422C7E70202}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividuallyFrom" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
     <t>/u01/app/oracle/product/12c/fwm/user_projects/domains/alfa/ear/parser/FProtegido</t>
   </si>
   <si>
-    <t>465O_11022021.xlsx</t>
+    <t>465O_12022021.xlsx</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>